<commit_message>
Added map stats + bug fixes
</commit_message>
<xml_diff>
--- a/mapsStats.xlsx
+++ b/mapsStats.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>teamId</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Heroic</t>
+  </si>
+  <si>
+    <t>Vitality</t>
   </si>
 </sst>
 </file>
@@ -420,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
@@ -496,6 +499,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9565</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>55.6</v>
+      </c>
+      <c r="D3">
+        <v>59.4</v>
+      </c>
+      <c r="E3">
+        <v>62.3</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>68.1</v>
+      </c>
+      <c r="H3">
+        <v>62.6</v>
+      </c>
+      <c r="I3">
+        <v>67.9</v>
+      </c>
+      <c r="J3">
+        <v>71.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>